<commit_message>
bf: update TAS3 froms
</commit_message>
<xml_diff>
--- a/LF/TAS/Burkina Faso/2024/oct/bf_lf_tas3_2410_2_participant.xlsx
+++ b/LF/TAS/Burkina Faso/2024/oct/bf_lf_tas3_2410_2_participant.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Burkina Faso\2024\jan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Burkina Faso\2024\oct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F77272A-FB56-478F-BF62-F6D34220B1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7F36F7-177A-4F7C-BBDF-C765B3A78281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1081,12 +1081,6 @@
     <t>2_nouvel_entrant</t>
   </si>
   <si>
-    <t>bf_lf_tas1_202401_2_participant_3</t>
-  </si>
-  <si>
-    <t>(Jan 2024) Burkina Faso TAS FL - 2. Formulaire Enrôlement V3</t>
-  </si>
-  <si>
     <t>1 Enregistré précédemment</t>
   </si>
   <si>
@@ -1100,6 +1094,12 @@
   </si>
   <si>
     <t>${status} = '1_enregistre_precedemment'</t>
+  </si>
+  <si>
+    <t>bf_lf_tas3_2410_2_participant</t>
+  </si>
+  <si>
+    <t>(Oct 2024) Burkina Faso TAS3 - 2. Formulaire Enrôlement</t>
   </si>
 </sst>
 </file>
@@ -2215,13 +2215,13 @@
         <v>167</v>
       </c>
       <c r="B25" t="s">
+        <v>345</v>
+      </c>
+      <c r="C25" t="s">
+        <v>346</v>
+      </c>
+      <c r="H25" t="s">
         <v>347</v>
-      </c>
-      <c r="C25" t="s">
-        <v>348</v>
-      </c>
-      <c r="H25" t="s">
-        <v>349</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>10</v>
@@ -3508,10 +3508,10 @@
         <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C62" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3999,7 +3999,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4021,10 +4021,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="B2" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="C2" t="s">
         <v>73</v>
@@ -4036,15 +4036,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F61D857ACC8084D9287671D8B7E15F4" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b2b3977cbccd3bcf631390164057ea08">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92042fd9-f4c9-49ed-97f1-ba485e322b1e" xmlns:ns3="744cc826-a471-4feb-879c-6424ce8a761f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e6655229457273daeac0ec2bc1901eb" ns2:_="" ns3:_="">
     <xsd:import namespace="92042fd9-f4c9-49ed-97f1-ba485e322b1e"/>
@@ -4273,15 +4264,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AA70DE9-52EB-4A74-A92B-6BC33DECE403}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7691146D-9A17-4B60-A330-159941DFBC25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4298,4 +4290,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AA70DE9-52EB-4A74-A92B-6BC33DECE403}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>